<commit_message>
Reading Modality, StudyDescription and StudyDate from DICOM files. Updated the fixture dicoms to have StudyDates matching the file patterns, and the fixture scan spreadsheet to have the correct DICOM parameters
</commit_message>
<xml_diff>
--- a/tests/fixtures/scanned.xlsx
+++ b/tests/fixtures/scanned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F641E6-0357-E24A-88B5-50F0EF48DF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379DF6DD-A00C-C840-A990-889E561E184E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9320" yWindow="8820" windowWidth="27780" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
   <si>
     <t>File</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>StudyDate</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>CT1 abdomen</t>
   </si>
 </sst>
 </file>
@@ -568,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -753,6 +759,15 @@
       <c r="G12" t="s">
         <v>29</v>
       </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
       <c r="K12" t="s">
         <v>30</v>
       </c>
@@ -802,6 +817,15 @@
       <c r="G14" t="s">
         <v>36</v>
       </c>
+      <c r="H14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
       <c r="K14" t="s">
         <v>30</v>
       </c>
@@ -862,6 +886,15 @@
       <c r="G17" t="s">
         <v>29</v>
       </c>
+      <c r="H17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
       <c r="K17" t="s">
         <v>42</v>
       </c>
@@ -933,6 +966,15 @@
       <c r="G21" t="s">
         <v>29</v>
       </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" t="s">
+        <v>48</v>
+      </c>
       <c r="K21" t="s">
         <v>49</v>
       </c>
@@ -993,6 +1035,15 @@
       <c r="G24" t="s">
         <v>29</v>
       </c>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
       <c r="K24" t="s">
         <v>49</v>
       </c>
@@ -1041,6 +1092,15 @@
       </c>
       <c r="G26" t="s">
         <v>29</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" t="s">
+        <v>61</v>
       </c>
       <c r="K26" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Updated scanned.xlsx in test fixtures to include SessionLabel column
</commit_message>
<xml_diff>
--- a/tests/fixtures/scanned.xlsx
+++ b/tests/fixtures/scanned.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379DF6DD-A00C-C840-A990-889E561E184E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4C4EBB-3A96-774E-81D8-04E45CE645E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9320" yWindow="8820" windowWidth="27780" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
   <si>
     <t>File</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>CT1 abdomen</t>
+  </si>
+  <si>
+    <t>SessionLabel</t>
   </si>
 </sst>
 </file>
@@ -572,15 +575,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -594,43 +597,46 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -641,7 +647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -652,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -663,7 +669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -674,7 +680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -685,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -696,7 +702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -707,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -718,7 +724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -729,7 +735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -740,7 +746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -750,44 +756,44 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>29</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>69</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>70</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>30</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>27</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>31</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>32</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>33</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -798,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -808,44 +814,44 @@
       <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>27</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>28</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>36</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>69</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>70</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>28</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>30</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>27</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>31</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>32</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>33</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -856,7 +862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -867,7 +873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -877,44 +883,44 @@
       <c r="C17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>41</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>29</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>69</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>70</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>41</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>42</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>40</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>31</v>
-      </c>
-      <c r="N17" t="s">
-        <v>32</v>
       </c>
       <c r="O17" t="s">
         <v>32</v>
       </c>
       <c r="P17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>43</v>
       </c>
@@ -925,7 +931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>44</v>
       </c>
@@ -936,7 +942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>45</v>
       </c>
@@ -947,7 +953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -957,44 +963,44 @@
       <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>47</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>48</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>69</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>70</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>48</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>49</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>47</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>50</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>51</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>52</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>53</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1026,44 +1032,44 @@
       <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>47</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>56</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>29</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>69</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>70</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>56</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>49</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>47</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>31</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>57</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>58</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1084,40 +1090,40 @@
       <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>47</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>61</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>29</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>69</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>70</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>61</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>49</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>47</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>62</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>63</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>64</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored DICOM parameters and how columns are written for values in dictionaries
</commit_message>
<xml_diff>
--- a/tests/fixtures/scanned.xlsx
+++ b/tests/fixtures/scanned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4C4EBB-3A96-774E-81D8-04E45CE645E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7EC379-12A9-FB4E-B270-88674FE04BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="8820" windowWidth="27780" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5500" yWindow="1240" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,10 +612,10 @@
         <v>66</v>
       </c>
       <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
         <v>67</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
@@ -769,10 +769,10 @@
         <v>69</v>
       </c>
       <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
         <v>70</v>
-      </c>
-      <c r="K12" t="s">
-        <v>28</v>
       </c>
       <c r="L12" t="s">
         <v>30</v>
@@ -827,10 +827,10 @@
         <v>69</v>
       </c>
       <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
         <v>70</v>
-      </c>
-      <c r="K14" t="s">
-        <v>28</v>
       </c>
       <c r="L14" t="s">
         <v>30</v>
@@ -896,10 +896,10 @@
         <v>69</v>
       </c>
       <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
         <v>70</v>
-      </c>
-      <c r="K17" t="s">
-        <v>41</v>
       </c>
       <c r="L17" t="s">
         <v>42</v>
@@ -976,10 +976,10 @@
         <v>69</v>
       </c>
       <c r="J21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" t="s">
         <v>70</v>
-      </c>
-      <c r="K21" t="s">
-        <v>48</v>
       </c>
       <c r="L21" t="s">
         <v>49</v>
@@ -1045,10 +1045,10 @@
         <v>69</v>
       </c>
       <c r="J24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" t="s">
         <v>70</v>
-      </c>
-      <c r="K24" t="s">
-        <v>56</v>
       </c>
       <c r="L24" t="s">
         <v>49</v>
@@ -1103,10 +1103,10 @@
         <v>69</v>
       </c>
       <c r="J26" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" t="s">
         <v>70</v>
-      </c>
-      <c r="K26" t="s">
-        <v>61</v>
       </c>
       <c r="L26" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Refactor to get matcher tests working again - also picked up a bug where it was scanning directories as well as files
</commit_message>
<xml_diff>
--- a/tests/fixtures/scanned.xlsx
+++ b/tests/fixtures/scanned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7EC379-12A9-FB4E-B270-88674FE04BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9584E6-1C33-E642-B056-85512E38F010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="1240" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13420" yWindow="3660" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
   <si>
     <t>File</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>tests/fixtures/source/NomatchDir</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -70,15 +67,6 @@
     <t>tests/fixtures/source/.DS_Store</t>
   </si>
   <si>
-    <t>tests/fixtures/source/DOE^JOHN-002304</t>
-  </si>
-  <si>
-    <t>tests/fixtures/source/Subdir</t>
-  </si>
-  <si>
-    <t>tests/fixtures/source/ROE^JANE-397829</t>
-  </si>
-  <si>
     <t>tests/fixtures/source/NomatchDir/no_match_file.txt</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
   </si>
   <si>
     <t>tests/fixtures/source/Subdir/.DS_Store</t>
-  </si>
-  <si>
-    <t>tests/fixtures/source/Subdir/Smith^John-038945</t>
   </si>
   <si>
     <t>tests/fixtures/source/Subdir/Smith^John-038945/20200303-scan1.dcm</t>
@@ -575,17 +560,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="46.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -597,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -609,13 +597,13 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
@@ -638,13 +626,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -652,10 +640,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -663,10 +651,10 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -674,10 +662,10 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -685,10 +673,10 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -696,435 +684,380 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" t="s">
+      <c r="O12" t="s">
         <v>28</v>
       </c>
-      <c r="H12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="P12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N12" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" t="s">
-        <v>32</v>
-      </c>
-      <c r="P12" t="s">
-        <v>33</v>
-      </c>
       <c r="Q12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J14" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L14" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" t="s">
-        <v>32</v>
-      </c>
-      <c r="P14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>36</v>
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" t="s">
-        <v>69</v>
-      </c>
-      <c r="J17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" t="s">
-        <v>40</v>
-      </c>
-      <c r="N17" t="s">
-        <v>31</v>
-      </c>
-      <c r="O17" t="s">
-        <v>32</v>
-      </c>
-      <c r="P17" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>29</v>
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
       <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
+      <c r="M19" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" t="s">
+        <v>52</v>
+      </c>
+      <c r="P19" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="K21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="L21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M21" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="N21" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="O21" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="P21" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" t="s">
-        <v>56</v>
-      </c>
-      <c r="K24" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24" t="s">
-        <v>49</v>
-      </c>
-      <c r="M24" t="s">
-        <v>47</v>
-      </c>
-      <c r="N24" t="s">
-        <v>31</v>
-      </c>
-      <c r="O24" t="s">
-        <v>57</v>
-      </c>
-      <c r="P24" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" t="s">
-        <v>69</v>
-      </c>
-      <c r="J26" t="s">
-        <v>61</v>
-      </c>
-      <c r="K26" t="s">
-        <v>70</v>
-      </c>
-      <c r="L26" t="s">
-        <v>49</v>
-      </c>
-      <c r="M26" t="s">
-        <v>47</v>
-      </c>
-      <c r="N26" t="s">
-        <v>62</v>
-      </c>
-      <c r="O26" t="s">
-        <v>63</v>
-      </c>
-      <c r="P26" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test fixtures to work with the new must-match-first-pattern style. Automatically ignore .DS_Store files, otherwise the tests will fail if they're run on a non-Mac
</commit_message>
<xml_diff>
--- a/tests/fixtures/scanned.xlsx
+++ b/tests/fixtures/scanned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9584E6-1C33-E642-B056-85512E38F010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0205D697-777D-E14B-B901-AC2255515606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="3660" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9440" yWindow="3080" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t>File</t>
   </si>
@@ -64,15 +64,9 @@
     <t>unmatched</t>
   </si>
   <si>
-    <t>tests/fixtures/source/.DS_Store</t>
-  </si>
-  <si>
     <t>tests/fixtures/source/NomatchDir/no_match_file.txt</t>
   </si>
   <si>
-    <t>tests/fixtures/source/DOE^JOHN-002304/.DS_Store</t>
-  </si>
-  <si>
     <t>tests/fixtures/source/DOE^JOHN-002304/20210430-scan1.txt</t>
   </si>
   <si>
@@ -121,12 +115,6 @@
     <t>scan2</t>
   </si>
   <si>
-    <t>tests/fixtures/source/Subdir/.DS_Store</t>
-  </si>
-  <si>
-    <t>tests/fixtures/source/Subdir/Smith^John-038945/20200303-scan1.dcm</t>
-  </si>
-  <si>
     <t>038945</t>
   </si>
   <si>
@@ -136,15 +124,6 @@
     <t>Smith^John</t>
   </si>
   <si>
-    <t>tests/fixtures/source/Subdir/Smith^John-038945/20200303-scan1.txt</t>
-  </si>
-  <si>
-    <t>tests/fixtures/source/Subdir/Smith^John-038945/no_match_file.txt</t>
-  </si>
-  <si>
-    <t>tests/fixtures/source/ROE^JANE-397829/.DS_Store</t>
-  </si>
-  <si>
     <t>tests/fixtures/source/ROE^JANE-397829/20190115-scan1.dcm</t>
   </si>
   <si>
@@ -221,6 +200,15 @@
   </si>
   <si>
     <t>SessionLabel</t>
+  </si>
+  <si>
+    <t>tests/fixtures/source/Smith^John-038945/20200303-scan1.dcm</t>
+  </si>
+  <si>
+    <t>tests/fixtures/source/Smith^John-038945/20200303-scan1.txt</t>
+  </si>
+  <si>
+    <t>tests/fixtures/source/Smith^John-038945/no_match_file.txt</t>
   </si>
 </sst>
 </file>
@@ -560,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,7 +561,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -585,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -597,13 +585,13 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
@@ -669,19 +657,55 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -692,112 +716,112 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" t="s">
         <v>25</v>
       </c>
-      <c r="I8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="O9" t="s">
         <v>26</v>
       </c>
-      <c r="M8" t="s">
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="s">
         <v>23</v>
       </c>
-      <c r="N8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" t="s">
-        <v>65</v>
-      </c>
-      <c r="L10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -808,13 +832,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>35</v>
@@ -823,16 +847,16 @@
         <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
         <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -841,21 +865,21 @@
         <v>35</v>
       </c>
       <c r="N12" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="O12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="P12" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="Q12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -866,7 +890,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -876,188 +900,108 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" t="s">
-        <v>65</v>
-      </c>
-      <c r="L16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M16" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O16" t="s">
-        <v>46</v>
-      </c>
-      <c r="P16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
       <c r="B17" t="s">
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="O17" t="s">
         <v>51</v>
       </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" t="s">
-        <v>44</v>
-      </c>
-      <c r="M19" t="s">
-        <v>42</v>
-      </c>
-      <c r="N19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="P17" t="s">
         <v>52</v>
       </c>
-      <c r="P19" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K21" t="s">
-        <v>65</v>
-      </c>
-      <c r="L21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M21" t="s">
-        <v>42</v>
-      </c>
-      <c r="N21" t="s">
-        <v>57</v>
-      </c>
-      <c r="O21" t="s">
-        <v>58</v>
-      </c>
-      <c r="P21" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>25</v>
+      <c r="Q17" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed collate_uploads so that it groups files by session:scan, not just session, and added tests and fixtures for this
</commit_message>
<xml_diff>
--- a/tests/fixtures/scanned.xlsx
+++ b/tests/fixtures/scanned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6A7B11-8919-4447-B961-926644EDA7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EB3582-CFA6-5C48-A7AC-E366C09C3134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="2620" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2000" yWindow="8520" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
   <si>
     <t>File</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>tests/fixtures/source/Smith^John-038945/20200303/X-Rays/20200303-scan1.txt</t>
+  </si>
+  <si>
+    <t>tests/fixtures/source/DOE^JOHN-002304/20200312/Chest CT/scan1.dcm</t>
+  </si>
+  <si>
+    <t>Chest_CT</t>
+  </si>
+  <si>
+    <t>20061012</t>
+  </si>
+  <si>
+    <t>Chest CT</t>
   </si>
 </sst>
 </file>
@@ -602,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S14"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,70 +686,70 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -745,10 +757,10 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -790,297 +802,336 @@
         <v>65</v>
       </c>
       <c r="S4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>44</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L7" t="s">
         <v>45</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M7" t="s">
         <v>29</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N7" t="s">
         <v>27</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O7" t="s">
         <v>30</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P7" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q7" t="s">
         <v>32</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R7" t="s">
         <v>5</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>71</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>33</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>5</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>44</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>33</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L9" t="s">
         <v>45</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>29</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N9" t="s">
         <v>27</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O9" t="s">
         <v>20</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P9" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q9" t="s">
         <v>35</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R9" t="s">
         <v>5</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>27</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>36</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>5</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>44</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>36</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>45</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>29</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N11" t="s">
         <v>27</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O11" t="s">
         <v>37</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P11" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q11" t="s">
         <v>39</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R11" t="s">
         <v>5</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>76</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>77</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>24</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>25</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>78</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>44</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>25</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>45</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>26</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N13" t="s">
         <v>24</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O13" t="s">
         <v>20</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P13" t="s">
         <v>21</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q13" t="s">
         <v>21</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R13" t="s">
         <v>78</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S13" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -1089,9 +1140,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:R17">
-    <sortCondition ref="B1:B17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:R18">
+    <sortCondition ref="B1:B18"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>